<commit_message>
feat(produits): mise à jour avancée de l'encodage des produits
</commit_message>
<xml_diff>
--- a/Ressources/Images/Produits/__Descriptions.xlsx
+++ b/Ressources/Images/Produits/__Descriptions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28725" windowHeight="5550"/>
+    <workbookView windowWidth="28800" windowHeight="12495"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1398,12 +1398,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1433,6 +1433,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1447,23 +1454,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1492,11 +1492,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1524,15 +1545,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1555,35 +1570,13 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1616,31 +1609,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1658,19 +1627,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1688,13 +1675,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1706,25 +1693,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1742,31 +1741,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1784,19 +1771,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1816,6 +1803,30 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -1844,16 +1855,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1867,17 +1878,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1896,193 +1903,168 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2135,7 +2117,7 @@
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="11">
     <dxf>
       <font>
         <name val="Calibri"/>
@@ -2232,6 +2214,22 @@
         <patternFill patternType="none"/>
       </fill>
     </dxf>
+    <dxf>
+      <font>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <u val="none"/>
+        <sz val="11"/>
+        <color theme="1"/>
+      </font>
+      <fill>
+        <patternFill patternType="none"/>
+      </fill>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -2256,7 +2254,7 @@
     <tableColumn id="8" name="RECAPITULATIF" dataDxfId="7"/>
     <tableColumn id="9" name="DESCRIPTION" dataDxfId="8"/>
     <tableColumn id="10" name="IMPACT PRIX" dataDxfId="9"/>
-    <tableColumn id="11" name="Column1"/>
+    <tableColumn id="11" name="Column1" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2522,8 +2520,8 @@
   <sheetPr/>
   <dimension ref="A1:L95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2570,13 +2568,13 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12"/>
+      <c r="L1" s="9"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="16.5" spans="1:12">
       <c r="A2" s="5" t="s">
@@ -2603,13 +2601,13 @@
       <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J2" s="5">
         <v>40</v>
       </c>
-      <c r="L2" s="14"/>
+      <c r="L2" s="11"/>
     </row>
     <row r="3" s="1" customFormat="1" spans="1:10">
       <c r="A3" s="5" t="s">
@@ -4027,1910 +4025,1910 @@
         <v>_Atari 7800 - Console - Bronze.jpg</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
-      <c r="A43" s="7" t="s">
+    <row r="43" s="1" customFormat="1" spans="1:11">
+      <c r="A43" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="B43" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E43" s="7" t="s">
+      <c r="E43" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="F43" s="8">
+      <c r="F43" s="5">
         <v>25</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="G43" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="H43" s="7" t="s">
+      <c r="H43" s="5" t="s">
         <v>210</v>
       </c>
-      <c r="I43" s="7" t="s">
+      <c r="I43" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="J43" s="7">
+      <c r="J43" s="5">
         <v>30</v>
       </c>
-      <c r="K43" t="str">
+      <c r="K43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Atari 7800 - Frenzy - Gold.jpg</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
-      <c r="A44" s="7" t="s">
+    <row r="44" s="1" customFormat="1" spans="1:11">
+      <c r="A44" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="B44" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="E44" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="F44" s="8">
+      <c r="F44" s="5">
         <v>35</v>
       </c>
-      <c r="G44" s="7" t="s">
+      <c r="G44" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="H44" s="7" t="s">
+      <c r="H44" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="I44" s="7" t="s">
+      <c r="I44" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="J44" s="7">
+      <c r="J44" s="5">
         <v>0</v>
       </c>
-      <c r="K44" t="str">
-        <f>_xlfn.CONCAT(G44,".jpg")</f>
+      <c r="K44" s="1" t="str">
+        <f t="shared" si="0"/>
         <v>Atari 7800 - Mario Bros - Silver.jpg</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
-      <c r="A45" s="7" t="s">
+    <row r="45" s="1" customFormat="1" spans="1:11">
+      <c r="A45" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="B45" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="E45" s="5" t="s">
         <v>218</v>
       </c>
-      <c r="F45" s="8">
+      <c r="F45" s="5">
         <v>20</v>
       </c>
-      <c r="G45" s="7" t="s">
+      <c r="G45" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="H45" s="7" t="s">
+      <c r="H45" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="I45" s="7" t="s">
+      <c r="I45" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="J45" s="7">
+      <c r="J45" s="5">
         <v>-10</v>
       </c>
-      <c r="K45" t="str">
+      <c r="K45" s="1" t="str">
         <f t="shared" ref="K45:K76" si="1">_xlfn.CONCAT(G45,".jpg")</f>
         <v>Atari 7800 - Choplifter - Bronze.jpg</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
-      <c r="A46" s="7" t="s">
+    <row r="46" s="1" customFormat="1" spans="1:11">
+      <c r="A46" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="B46" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C46" s="7" t="s">
+      <c r="C46" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E46" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="F46" s="8">
+      <c r="F46" s="5">
         <v>150</v>
       </c>
-      <c r="G46" s="7" t="s">
+      <c r="G46" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="H46" s="7" t="s">
+      <c r="H46" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="I46" s="7" t="s">
+      <c r="I46" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="J46" s="7">
+      <c r="J46" s="5">
         <v>50</v>
       </c>
-      <c r="K46" t="str">
+      <c r="K46" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_GX-4000 - Console - Gold.jpg.jpg</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
-      <c r="A47" s="7" t="s">
+    <row r="47" s="1" customFormat="1" spans="1:11">
+      <c r="A47" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E47" s="7" t="s">
+      <c r="E47" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="F47" s="8">
+      <c r="F47" s="5">
         <v>35</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G47" s="5" t="s">
         <v>230</v>
       </c>
-      <c r="H47" s="7" t="s">
+      <c r="H47" s="5" t="s">
         <v>231</v>
       </c>
-      <c r="I47" s="7" t="s">
+      <c r="I47" s="5" t="s">
         <v>232</v>
       </c>
-      <c r="J47" s="7">
+      <c r="J47" s="5">
         <v>25</v>
       </c>
-      <c r="K47" t="str">
+      <c r="K47" s="1" t="str">
         <f t="shared" si="1"/>
         <v>GX-4000 - Navy Seals - Gold.jpg</v>
       </c>
     </row>
-    <row r="48" spans="1:11">
-      <c r="A48" s="7" t="s">
+    <row r="48" s="1" customFormat="1" spans="1:11">
+      <c r="A48" s="5" t="s">
         <v>233</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="C48" s="7" t="s">
+      <c r="C48" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="E48" s="5" t="s">
         <v>234</v>
       </c>
-      <c r="F48" s="8">
+      <c r="F48" s="5">
         <v>35</v>
       </c>
-      <c r="G48" s="7" t="s">
+      <c r="G48" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="H48" s="7" t="s">
+      <c r="H48" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="I48" s="7" t="s">
+      <c r="I48" s="5" t="s">
         <v>237</v>
       </c>
-      <c r="J48" s="7">
+      <c r="J48" s="5">
         <v>25</v>
       </c>
-      <c r="K48" t="str">
+      <c r="K48" s="1" t="str">
         <f t="shared" si="1"/>
         <v>GX-4000 - Switch Blade - Gold.jpg</v>
       </c>
     </row>
-    <row r="49" spans="1:11">
-      <c r="A49" s="7" t="s">
+    <row r="49" s="1" customFormat="1" spans="1:11">
+      <c r="A49" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="E49" s="5" t="s">
         <v>241</v>
       </c>
-      <c r="F49" s="8">
+      <c r="F49" s="5">
         <v>350</v>
       </c>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="7" t="s">
         <v>242</v>
       </c>
-      <c r="H49" s="7" t="s">
+      <c r="H49" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="I49" s="7" t="s">
+      <c r="I49" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="J49" s="7">
+      <c r="J49" s="5">
         <v>-100</v>
       </c>
-      <c r="K49" t="str">
+      <c r="K49" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_CD-I - Console - Bronze.jpg</v>
       </c>
     </row>
-    <row r="50" spans="1:11">
-      <c r="A50" s="7" t="s">
+    <row r="50" s="1" customFormat="1" spans="1:11">
+      <c r="A50" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="B50" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E50" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="F50" s="8">
+      <c r="F50" s="5">
         <v>350</v>
       </c>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="7" t="s">
         <v>246</v>
       </c>
-      <c r="H50" s="7" t="s">
+      <c r="H50" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="I50" s="7" t="s">
+      <c r="I50" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="J50" s="7">
+      <c r="J50" s="5">
         <v>0</v>
       </c>
-      <c r="K50" t="str">
+      <c r="K50" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_CD-I - Console - Silver.jpg</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
-      <c r="A51" s="7" t="s">
+    <row r="51" s="1" customFormat="1" spans="1:11">
+      <c r="A51" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="B51" s="7" t="s">
+      <c r="B51" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E51" s="7" t="s">
+      <c r="E51" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="F51" s="8">
+      <c r="F51" s="5">
         <v>80</v>
       </c>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="7" t="s">
         <v>249</v>
       </c>
-      <c r="H51" s="9" t="s">
+      <c r="H51" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="I51" s="7" t="s">
+      <c r="I51" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="J51" s="7">
+      <c r="J51" s="5">
         <v>20</v>
       </c>
-      <c r="K51" t="str">
+      <c r="K51" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CD-I - Zelda The Wand Of Gamelon - Gold.jpg</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
-      <c r="A52" s="7" t="s">
+    <row r="52" s="1" customFormat="1" spans="1:11">
+      <c r="A52" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="B52" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="C52" s="7" t="s">
+      <c r="C52" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E52" s="7" t="s">
+      <c r="E52" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="F52" s="8">
+      <c r="F52" s="5">
         <v>80</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="7" t="s">
         <v>254</v>
       </c>
-      <c r="H52" s="9" t="s">
+      <c r="H52" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="I52" s="7" t="s">
+      <c r="I52" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="J52" s="7">
+      <c r="J52" s="5">
         <v>20</v>
       </c>
-      <c r="K52" t="str">
+      <c r="K52" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CD-I - Zelda's Adventure - Gold.jpg</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
-      <c r="A53" s="7" t="s">
+    <row r="53" s="1" customFormat="1" spans="1:11">
+      <c r="A53" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B53" s="9" t="s">
+      <c r="B53" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E53" s="9" t="s">
+      <c r="E53" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="F53" s="10">
+      <c r="F53" s="7">
         <v>250</v>
       </c>
-      <c r="G53" s="9" t="s">
+      <c r="G53" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="H53" s="7" t="s">
+      <c r="H53" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="I53" s="7" t="s">
+      <c r="I53" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="J53" s="9">
+      <c r="J53" s="7">
         <v>80</v>
       </c>
-      <c r="K53" t="str">
+      <c r="K53" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_MegaDrive - Console - Gold.jpg</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
-      <c r="A54" s="7" t="s">
+    <row r="54" s="1" customFormat="1" spans="1:11">
+      <c r="A54" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="9" t="s">
+      <c r="E54" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="F54" s="10">
+      <c r="F54" s="7">
         <v>250</v>
       </c>
-      <c r="G54" s="9" t="s">
+      <c r="G54" s="7" t="s">
         <v>264</v>
       </c>
-      <c r="H54" s="7" t="s">
+      <c r="H54" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="I54" s="7" t="s">
+      <c r="I54" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="J54" s="9">
+      <c r="J54" s="7">
         <v>-100</v>
       </c>
-      <c r="K54" t="str">
+      <c r="K54" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_MegaDrive - Console - Bronze.jpg</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
-      <c r="A55" s="7" t="s">
+    <row r="55" s="1" customFormat="1" spans="1:11">
+      <c r="A55" s="5" t="s">
         <v>265</v>
       </c>
-      <c r="B55" s="9" t="s">
+      <c r="B55" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E55" s="9" t="s">
+      <c r="E55" s="7" t="s">
         <v>266</v>
       </c>
-      <c r="F55" s="10">
+      <c r="F55" s="7">
         <v>350</v>
       </c>
-      <c r="G55" s="9" t="s">
+      <c r="G55" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="H55" s="7" t="s">
+      <c r="H55" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="I55" s="7" t="s">
+      <c r="I55" s="5" t="s">
         <v>269</v>
       </c>
-      <c r="J55" s="9">
+      <c r="J55" s="7">
         <v>80</v>
       </c>
-      <c r="K55" t="str">
+      <c r="K55" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_MegaDrive 2 - Console - Gold.jpg</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
-      <c r="A56" s="7" t="s">
+    <row r="56" s="1" customFormat="1" spans="1:11">
+      <c r="A56" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="B56" s="9" t="s">
+      <c r="B56" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E56" s="9" t="s">
+      <c r="E56" s="7" t="s">
         <v>271</v>
       </c>
-      <c r="F56" s="10">
+      <c r="F56" s="7">
         <v>65</v>
       </c>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="H56" s="9" t="s">
+      <c r="H56" s="7" t="s">
         <v>273</v>
       </c>
-      <c r="I56" s="7" t="s">
+      <c r="I56" s="5" t="s">
         <v>274</v>
       </c>
-      <c r="J56" s="9">
+      <c r="J56" s="7">
         <v>30</v>
       </c>
-      <c r="K56" t="str">
+      <c r="K56" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MegaDrive - Mega Turrican - Gold.jpg</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
-      <c r="A57" s="7" t="s">
+    <row r="57" s="1" customFormat="1" spans="1:11">
+      <c r="A57" s="5" t="s">
         <v>275</v>
       </c>
-      <c r="B57" s="9" t="s">
+      <c r="B57" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E57" s="9" t="s">
+      <c r="E57" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="F57" s="10">
+      <c r="F57" s="7">
         <v>65</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G57" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="H57" s="9" t="s">
+      <c r="H57" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="I57" s="9" t="s">
+      <c r="I57" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="J57" s="9">
+      <c r="J57" s="7">
         <v>30</v>
       </c>
-      <c r="K57" t="str">
+      <c r="K57" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MegaDrive - Comix Zone - Gold.jpg</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
-      <c r="A58" s="7" t="s">
+    <row r="58" s="1" customFormat="1" spans="1:11">
+      <c r="A58" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="B58" s="9" t="s">
+      <c r="B58" s="7" t="s">
         <v>258</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E58" s="9" t="s">
+      <c r="E58" s="7" t="s">
         <v>281</v>
       </c>
-      <c r="F58" s="10">
+      <c r="F58" s="7">
         <v>70</v>
       </c>
-      <c r="G58" s="9" t="s">
+      <c r="G58" s="7" t="s">
         <v>282</v>
       </c>
-      <c r="H58" s="9" t="s">
+      <c r="H58" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="I58" s="9" t="s">
+      <c r="I58" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="J58" s="9">
+      <c r="J58" s="7">
         <v>30</v>
       </c>
-      <c r="K58" t="str">
+      <c r="K58" s="1" t="str">
         <f t="shared" si="1"/>
         <v>MegaDrive - Robocop 3 - Gold.jpg</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
-      <c r="A59" s="7" t="s">
+    <row r="59" s="1" customFormat="1" spans="1:11">
+      <c r="A59" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B59" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E59" s="9" t="s">
+      <c r="E59" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="F59" s="10">
+      <c r="F59" s="7">
         <v>400</v>
       </c>
-      <c r="G59" s="9" t="s">
+      <c r="G59" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="H59" s="7" t="s">
+      <c r="H59" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="I59" s="7" t="s">
+      <c r="I59" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="J59" s="9">
+      <c r="J59" s="7">
         <v>-150</v>
       </c>
-      <c r="K59" t="str">
+      <c r="K59" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_Neo-Geo - Console - Bronze.jpg</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
-      <c r="A60" s="7" t="s">
+    <row r="60" s="1" customFormat="1" spans="1:11">
+      <c r="A60" s="5" t="s">
         <v>285</v>
       </c>
-      <c r="B60" s="9" t="s">
+      <c r="B60" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E60" s="9" t="s">
+      <c r="E60" s="7" t="s">
         <v>291</v>
       </c>
-      <c r="F60" s="10">
+      <c r="F60" s="7">
         <v>400</v>
       </c>
-      <c r="G60" s="9" t="s">
+      <c r="G60" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="H60" s="7" t="s">
+      <c r="H60" s="5" t="s">
         <v>289</v>
       </c>
-      <c r="I60" s="7" t="s">
+      <c r="I60" s="5" t="s">
         <v>290</v>
       </c>
-      <c r="J60" s="9">
+      <c r="J60" s="7">
         <v>500</v>
       </c>
-      <c r="K60" t="str">
+      <c r="K60" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_Neo-Geo - Console - Platinum.jpg</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
-      <c r="A61" s="7" t="s">
+    <row r="61" s="1" customFormat="1" spans="1:11">
+      <c r="A61" s="5" t="s">
         <v>293</v>
       </c>
-      <c r="B61" s="9" t="s">
+      <c r="B61" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E61" s="9" t="s">
+      <c r="E61" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="F61" s="10">
+      <c r="F61" s="7">
         <v>125</v>
       </c>
-      <c r="G61" s="9" t="s">
+      <c r="G61" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="H61" s="9" t="s">
+      <c r="H61" s="7" t="s">
         <v>296</v>
       </c>
-      <c r="I61" s="9" t="s">
+      <c r="I61" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="J61" s="9">
+      <c r="J61" s="7">
         <v>40</v>
       </c>
-      <c r="K61" t="str">
+      <c r="K61" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Neo-Geo - Metal Slug - Gold.jpg</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
-      <c r="A62" s="7" t="s">
+    <row r="62" s="1" customFormat="1" spans="1:11">
+      <c r="A62" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="B62" s="9" t="s">
+      <c r="B62" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E62" s="9" t="s">
+      <c r="E62" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="F62" s="10">
+      <c r="F62" s="7">
         <v>120</v>
       </c>
-      <c r="G62" s="9" t="s">
+      <c r="G62" s="7" t="s">
         <v>300</v>
       </c>
-      <c r="H62" s="9" t="s">
+      <c r="H62" s="7" t="s">
         <v>301</v>
       </c>
-      <c r="I62" s="9" t="s">
+      <c r="I62" s="7" t="s">
         <v>302</v>
       </c>
-      <c r="J62" s="9">
+      <c r="J62" s="7">
         <v>40</v>
       </c>
-      <c r="K62" t="str">
+      <c r="K62" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Neo-Geo - Metal Slug 3 - Gold.jpg</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
-      <c r="A63" s="7" t="s">
+    <row r="63" s="1" customFormat="1" spans="1:11">
+      <c r="A63" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="B63" s="9" t="s">
+      <c r="B63" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E63" s="9" t="s">
+      <c r="E63" s="7" t="s">
         <v>304</v>
       </c>
-      <c r="F63" s="10">
+      <c r="F63" s="7">
         <v>250</v>
       </c>
-      <c r="G63" s="9" t="s">
+      <c r="G63" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="H63" s="9" t="s">
+      <c r="H63" s="7" t="s">
         <v>306</v>
       </c>
-      <c r="I63" s="9" t="s">
+      <c r="I63" s="7" t="s">
         <v>307</v>
       </c>
-      <c r="J63" s="9">
+      <c r="J63" s="7">
         <v>125</v>
       </c>
-      <c r="K63" t="str">
+      <c r="K63" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Neo-Geo - WindJammers - Platinum.jpg</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
-      <c r="A64" s="7" t="s">
+    <row r="64" s="1" customFormat="1" spans="1:11">
+      <c r="A64" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B64" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E64" s="9" t="s">
+      <c r="E64" s="7" t="s">
         <v>310</v>
       </c>
-      <c r="F64" s="10">
+      <c r="F64" s="7">
         <v>300</v>
       </c>
-      <c r="G64" s="9" t="s">
+      <c r="G64" s="7" t="s">
         <v>311</v>
       </c>
-      <c r="H64" s="7" t="s">
+      <c r="H64" s="5" t="s">
         <v>312</v>
       </c>
-      <c r="I64" s="7" t="s">
+      <c r="I64" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="J64" s="7">
+      <c r="J64" s="5">
         <v>0</v>
       </c>
-      <c r="K64" t="str">
+      <c r="K64" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_SNES - Console - Silver.jpg</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
-      <c r="A65" s="7" t="s">
+    <row r="65" s="1" customFormat="1" spans="1:11">
+      <c r="A65" s="5" t="s">
         <v>314</v>
       </c>
-      <c r="B65" s="9" t="s">
+      <c r="B65" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E65" s="9" t="s">
+      <c r="E65" s="7" t="s">
         <v>315</v>
       </c>
-      <c r="F65" s="10">
+      <c r="F65" s="7">
         <v>80</v>
       </c>
-      <c r="G65" s="9" t="s">
+      <c r="G65" s="7" t="s">
         <v>316</v>
       </c>
-      <c r="H65" s="9" t="s">
+      <c r="H65" s="7" t="s">
         <v>317</v>
       </c>
-      <c r="I65" s="7" t="s">
+      <c r="I65" s="5" t="s">
         <v>318</v>
       </c>
-      <c r="J65" s="7">
+      <c r="J65" s="5">
         <v>0</v>
       </c>
-      <c r="K65" t="str">
+      <c r="K65" s="1" t="str">
         <f t="shared" si="1"/>
         <v>SNES - Aladdin - Silver.jpg</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
-      <c r="A66" s="7" t="s">
+    <row r="66" s="1" customFormat="1" spans="1:11">
+      <c r="A66" s="5" t="s">
         <v>319</v>
       </c>
-      <c r="B66" s="9" t="s">
+      <c r="B66" s="7" t="s">
         <v>309</v>
       </c>
-      <c r="C66" s="7" t="s">
+      <c r="C66" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E66" s="9" t="s">
+      <c r="E66" s="7" t="s">
         <v>320</v>
       </c>
-      <c r="F66" s="10">
+      <c r="F66" s="7">
         <v>100</v>
       </c>
-      <c r="G66" s="9" t="s">
+      <c r="G66" s="7" t="s">
         <v>321</v>
       </c>
-      <c r="H66" s="9" t="s">
+      <c r="H66" s="7" t="s">
         <v>322</v>
       </c>
-      <c r="I66" s="7" t="s">
+      <c r="I66" s="5" t="s">
         <v>323</v>
       </c>
-      <c r="J66" s="9">
+      <c r="J66" s="7">
         <v>-50</v>
       </c>
-      <c r="K66" t="str">
+      <c r="K66" s="1" t="str">
         <f t="shared" si="1"/>
         <v>SNES - Super Ghouls 'n Ghosts - Bronze.jpg</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
-      <c r="A67" s="15" t="s">
+    <row r="67" s="1" customFormat="1" spans="1:11">
+      <c r="A67" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="B67" s="16" t="s">
+      <c r="B67" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C67" s="7" t="s">
+      <c r="C67" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D67" s="7" t="s">
+      <c r="D67" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E67" s="16" t="s">
+      <c r="E67" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="F67" s="17">
+      <c r="F67" s="1">
         <v>50</v>
       </c>
-      <c r="G67" s="16" t="s">
+      <c r="G67" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="H67" s="16" t="s">
+      <c r="H67" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="I67" s="15" t="s">
+      <c r="I67" s="12" t="s">
         <v>330</v>
       </c>
-      <c r="J67" s="16">
+      <c r="J67" s="1">
         <v>25</v>
       </c>
-      <c r="K67" t="str">
+      <c r="K67" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Jaguar - Doom - Gold.jpg</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
-      <c r="A68" s="15" t="s">
+    <row r="68" s="1" customFormat="1" spans="1:11">
+      <c r="A68" s="12" t="s">
         <v>331</v>
       </c>
-      <c r="B68" s="16" t="s">
+      <c r="B68" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C68" s="7" t="s">
+      <c r="C68" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E68" s="16" t="s">
+      <c r="E68" s="1" t="s">
         <v>332</v>
       </c>
-      <c r="F68" s="17">
+      <c r="F68" s="1">
         <v>40</v>
       </c>
-      <c r="G68" s="16" t="s">
+      <c r="G68" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="H68" s="16" t="s">
+      <c r="H68" s="1" t="s">
         <v>334</v>
       </c>
-      <c r="I68" s="15" t="s">
+      <c r="I68" s="12" t="s">
         <v>335</v>
       </c>
-      <c r="J68" s="7">
+      <c r="J68" s="5">
         <v>0</v>
       </c>
-      <c r="K68" t="str">
+      <c r="K68" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Jaguar - Flashback - Silver.jpg</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
-      <c r="A69" s="15" t="s">
+    <row r="69" s="1" customFormat="1" spans="1:11">
+      <c r="A69" s="12" t="s">
         <v>336</v>
       </c>
-      <c r="B69" s="16" t="s">
+      <c r="B69" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="C69" s="7" t="s">
+      <c r="C69" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="E69" s="1" t="s">
         <v>337</v>
       </c>
-      <c r="F69" s="17">
+      <c r="F69" s="1">
         <v>40</v>
       </c>
-      <c r="G69" s="16" t="s">
+      <c r="G69" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="H69" s="16" t="s">
+      <c r="H69" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="I69" s="15" t="s">
+      <c r="I69" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="J69" s="16">
+      <c r="J69" s="1">
         <v>-25</v>
       </c>
-      <c r="K69" t="str">
+      <c r="K69" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Jaguar - Missile Command 3D - Bronze.jpg</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
-      <c r="A70" s="15" t="s">
+    <row r="70" s="1" customFormat="1" spans="1:11">
+      <c r="A70" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="B70" s="16" t="s">
+      <c r="B70" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C70" s="7" t="s">
+      <c r="C70" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E70" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="F70" s="17">
+      <c r="F70" s="1">
         <v>250</v>
       </c>
-      <c r="G70" s="16" t="s">
+      <c r="G70" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="H70" s="16" t="s">
+      <c r="H70" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="I70" s="15" t="s">
+      <c r="I70" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="J70" s="7">
+      <c r="J70" s="5">
         <v>0</v>
       </c>
-      <c r="K70" t="str">
+      <c r="K70" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_N64 - Console - Silver.jpg</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
-      <c r="A71" s="15" t="s">
+    <row r="71" s="1" customFormat="1" spans="1:11">
+      <c r="A71" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="B71" s="16" t="s">
+      <c r="B71" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="C71" s="7" t="s">
+      <c r="C71" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E71" s="16" t="s">
+      <c r="E71" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="F71" s="17">
+      <c r="F71" s="1">
         <v>250</v>
       </c>
-      <c r="G71" s="16" t="s">
+      <c r="G71" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="H71" s="16" t="s">
+      <c r="H71" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="I71" s="15" t="s">
+      <c r="I71" s="12" t="s">
         <v>346</v>
       </c>
-      <c r="J71" s="16">
+      <c r="J71" s="1">
         <v>80</v>
       </c>
-      <c r="K71" t="str">
+      <c r="K71" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_N64 - Console - Gold.jpg</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
-      <c r="A72" s="15" t="s">
+    <row r="72" s="1" customFormat="1" spans="1:11">
+      <c r="A72" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="B72" s="16" t="s">
+      <c r="B72" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C72" s="7" t="s">
+      <c r="C72" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E72" s="16" t="s">
+      <c r="E72" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="F72" s="17">
+      <c r="F72" s="1">
         <v>250</v>
       </c>
-      <c r="G72" s="16" t="s">
+      <c r="G72" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="H72" s="16" t="s">
+      <c r="H72" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="I72" s="15" t="s">
+      <c r="I72" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="J72" s="16">
+      <c r="J72" s="1">
         <v>50</v>
       </c>
-      <c r="K72" t="str">
+      <c r="K72" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_Playstation 1 - Console - Gold.jpg</v>
       </c>
     </row>
-    <row r="73" spans="1:11">
-      <c r="A73" s="15" t="s">
+    <row r="73" s="1" customFormat="1" spans="1:11">
+      <c r="A73" s="12" t="s">
         <v>349</v>
       </c>
-      <c r="B73" s="16" t="s">
+      <c r="B73" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C73" s="7" t="s">
+      <c r="C73" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D73" s="7" t="s">
+      <c r="D73" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E73" s="16" t="s">
+      <c r="E73" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="F73" s="17">
+      <c r="F73" s="1">
         <v>250</v>
       </c>
-      <c r="G73" s="16" t="s">
+      <c r="G73" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="H73" s="16" t="s">
+      <c r="H73" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="I73" s="15" t="s">
+      <c r="I73" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="J73" s="16">
+      <c r="J73" s="1">
         <v>-120</v>
       </c>
-      <c r="K73" t="str">
+      <c r="K73" s="1" t="str">
         <f t="shared" si="1"/>
         <v>_Playstation 1 - Console - Bronze.jpg</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
-      <c r="A74" s="15" t="s">
+    <row r="74" s="1" customFormat="1" spans="1:11">
+      <c r="A74" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C74" s="7" t="s">
+      <c r="C74" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D74" s="7" t="s">
+      <c r="D74" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="F74" s="17">
+      <c r="F74" s="1">
         <v>50</v>
       </c>
-      <c r="G74" s="16" t="s">
+      <c r="G74" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="H74" s="16" t="s">
+      <c r="H74" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="I74" s="15" t="s">
+      <c r="I74" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="J74" s="16">
+      <c r="J74" s="1">
         <v>35</v>
       </c>
-      <c r="K74" t="str">
+      <c r="K74" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Playstation 1 - Hercule - Bronze.jpg</v>
       </c>
     </row>
-    <row r="75" spans="1:11">
-      <c r="A75" s="15" t="s">
+    <row r="75" s="1" customFormat="1" spans="1:11">
+      <c r="A75" s="12" t="s">
         <v>357</v>
       </c>
-      <c r="B75" s="16" t="s">
+      <c r="B75" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C75" s="7" t="s">
+      <c r="C75" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D75" s="7" t="s">
+      <c r="D75" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E75" s="16" t="s">
+      <c r="E75" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="F75" s="17">
+      <c r="F75" s="1">
         <v>50</v>
       </c>
-      <c r="G75" s="16" t="s">
+      <c r="G75" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="H75" s="16" t="s">
+      <c r="H75" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="I75" s="15" t="s">
+      <c r="I75" s="12" t="s">
         <v>361</v>
       </c>
-      <c r="J75" s="16">
+      <c r="J75" s="1">
         <v>35</v>
       </c>
-      <c r="K75" t="str">
+      <c r="K75" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Playstation 1 - Hercule - Gold.jpg</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
-      <c r="A76" s="15" t="s">
+    <row r="76" s="1" customFormat="1" spans="1:11">
+      <c r="A76" s="12" t="s">
         <v>364</v>
       </c>
-      <c r="B76" s="16" t="s">
+      <c r="B76" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C76" s="7" t="s">
+      <c r="C76" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D76" s="7" t="s">
+      <c r="D76" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E76" s="16" t="s">
+      <c r="E76" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="F76" s="17">
+      <c r="F76" s="1">
         <v>80</v>
       </c>
-      <c r="G76" s="16" t="s">
+      <c r="G76" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="H76" s="16" t="s">
+      <c r="H76" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="I76" s="15" t="s">
+      <c r="I76" s="12" t="s">
         <v>368</v>
       </c>
-      <c r="J76" s="16">
+      <c r="J76" s="1">
         <v>40</v>
       </c>
-      <c r="K76" t="str">
+      <c r="K76" s="1" t="str">
         <f t="shared" si="1"/>
         <v>Playstation 1 - Suikoden - Gold.jpg</v>
       </c>
     </row>
-    <row r="77" spans="1:11">
-      <c r="A77" s="15" t="s">
+    <row r="77" s="1" customFormat="1" spans="1:11">
+      <c r="A77" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="B77" s="16" t="s">
+      <c r="B77" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C77" s="7" t="s">
+      <c r="C77" s="5" t="s">
         <v>326</v>
       </c>
-      <c r="D77" s="7" t="s">
+      <c r="D77" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="F77" s="17">
+      <c r="F77" s="1">
         <v>100</v>
       </c>
-      <c r="G77" s="16" t="s">
+      <c r="G77" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="H77" s="16" t="s">
+      <c r="H77" s="1" t="s">
         <v>372</v>
       </c>
-      <c r="I77" s="15" t="s">
+      <c r="I77" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="J77" s="7">
+      <c r="J77" s="5">
         <v>0</v>
       </c>
-      <c r="K77" t="str">
+      <c r="K77" s="1" t="str">
         <f t="shared" ref="K77:K95" si="2">_xlfn.CONCAT(G77,".jpg")</f>
         <v>Playstation 1 - Final Fantasy VIII - Silver.jpg</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
-      <c r="A78" s="15" t="s">
+    <row r="78" s="1" customFormat="1" spans="1:11">
+      <c r="A78" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="B78" s="16" t="s">
+      <c r="B78" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C78" s="7" t="s">
+      <c r="C78" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D78" s="7" t="s">
+      <c r="D78" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E78" s="16" t="s">
+      <c r="E78" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="F78" s="17">
+      <c r="F78" s="1">
         <v>180</v>
       </c>
-      <c r="G78" s="16" t="s">
+      <c r="G78" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="H78" s="16" t="s">
+      <c r="H78" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="I78" s="15" t="s">
+      <c r="I78" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="J78" s="16">
+      <c r="J78" s="1">
         <v>-80</v>
       </c>
-      <c r="K78" t="str">
+      <c r="K78" s="1" t="str">
         <f t="shared" si="2"/>
         <v>_Dreamcast - Console - Bronze.jpg</v>
       </c>
     </row>
-    <row r="79" spans="1:11">
-      <c r="A79" s="15" t="s">
+    <row r="79" s="1" customFormat="1" spans="1:11">
+      <c r="A79" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C79" s="7" t="s">
+      <c r="C79" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D79" s="7" t="s">
+      <c r="D79" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E79" s="16" t="s">
+      <c r="E79" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="F79" s="17">
+      <c r="F79" s="1">
         <v>180</v>
       </c>
-      <c r="G79" s="16" t="s">
+      <c r="G79" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="H79" s="16" t="s">
+      <c r="H79" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="I79" s="15" t="s">
+      <c r="I79" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="J79" s="16">
+      <c r="J79" s="1">
         <v>50</v>
       </c>
-      <c r="K79" t="str">
+      <c r="K79" s="1" t="str">
         <f t="shared" si="2"/>
         <v>_Dreamcast - Console - Gold.jpg</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
-      <c r="A80" s="15" t="s">
+    <row r="80" s="1" customFormat="1" spans="1:11">
+      <c r="A80" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C80" s="7" t="s">
+      <c r="C80" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E80" s="16" t="s">
+      <c r="E80" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="F80" s="17">
+      <c r="F80" s="1">
         <v>45</v>
       </c>
-      <c r="G80" s="16" t="s">
+      <c r="G80" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="H80" s="16" t="s">
+      <c r="H80" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="I80" s="15" t="s">
+      <c r="I80" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="J80" s="16">
+      <c r="J80" s="1">
         <v>80</v>
       </c>
-      <c r="K80" t="str">
+      <c r="K80" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Dreamcast - ChuChu Rocket - Platinum.jpg</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
-      <c r="A81" s="15" t="s">
+    <row r="81" s="1" customFormat="1" spans="1:11">
+      <c r="A81" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C81" s="7" t="s">
+      <c r="C81" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D81" s="7" t="s">
+      <c r="D81" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E81" s="16" t="s">
+      <c r="E81" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="F81" s="17">
+      <c r="F81" s="1">
         <v>45</v>
       </c>
-      <c r="G81" s="16" t="s">
+      <c r="G81" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="H81" s="16" t="s">
+      <c r="H81" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="I81" s="15" t="s">
+      <c r="I81" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="J81" s="16">
+      <c r="J81" s="1">
         <v>-25</v>
       </c>
-      <c r="K81" t="str">
+      <c r="K81" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Dreamcast - Worms Armageddon - Bronze.jpg</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
-      <c r="A82" s="15" t="s">
+    <row r="82" s="1" customFormat="1" spans="1:11">
+      <c r="A82" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C82" s="7" t="s">
+      <c r="C82" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D82" s="7" t="s">
+      <c r="D82" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="E82" s="1" t="s">
         <v>394</v>
       </c>
-      <c r="F82" s="17">
+      <c r="F82" s="1">
         <v>75</v>
       </c>
-      <c r="G82" s="16" t="s">
+      <c r="G82" s="1" t="s">
         <v>395</v>
       </c>
-      <c r="H82" s="16" t="s">
+      <c r="H82" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="I82" s="15" t="s">
+      <c r="I82" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="J82" s="16">
+      <c r="J82" s="1">
         <v>25</v>
       </c>
-      <c r="K82" t="str">
+      <c r="K82" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Dreamcast - Sonic Adventure - Gold.jpg</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
-      <c r="A83" s="15" t="s">
+    <row r="83" s="1" customFormat="1" spans="1:11">
+      <c r="A83" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C83" s="7" t="s">
+      <c r="C83" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D83" s="7" t="s">
+      <c r="D83" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="E83" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="F83" s="17">
+      <c r="F83" s="1">
         <v>75</v>
       </c>
-      <c r="G83" s="16" t="s">
+      <c r="G83" s="1" t="s">
         <v>400</v>
       </c>
-      <c r="H83" s="16" t="s">
+      <c r="H83" s="1" t="s">
         <v>401</v>
       </c>
-      <c r="I83" s="15" t="s">
+      <c r="I83" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="J83" s="16">
+      <c r="J83" s="1">
         <v>-25</v>
       </c>
-      <c r="K83" t="str">
+      <c r="K83" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Dreamcast - Rayman 2 - Bronze.jpg</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
-      <c r="A84" s="15" t="s">
+    <row r="84" s="1" customFormat="1" spans="1:11">
+      <c r="A84" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C84" s="7" t="s">
+      <c r="C84" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D84" s="7" t="s">
+      <c r="D84" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="E84" s="1" t="s">
         <v>404</v>
       </c>
-      <c r="F84" s="17">
+      <c r="F84" s="1">
         <v>80</v>
       </c>
-      <c r="G84" s="16" t="s">
+      <c r="G84" s="1" t="s">
         <v>405</v>
       </c>
-      <c r="H84" s="16" t="s">
+      <c r="H84" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="I84" s="15" t="s">
+      <c r="I84" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="J84" s="16">
+      <c r="J84" s="1">
         <v>30</v>
       </c>
-      <c r="K84" t="str">
+      <c r="K84" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Dreamcast - Resident Evil 2 - Gold.jpg</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
-      <c r="A85" s="15" t="s">
+    <row r="85" s="1" customFormat="1" spans="1:11">
+      <c r="A85" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="C85" s="7" t="s">
+      <c r="C85" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D85" s="7" t="s">
+      <c r="D85" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="E85" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="F85" s="17">
+      <c r="F85" s="1">
         <v>95</v>
       </c>
-      <c r="G85" s="16" t="s">
+      <c r="G85" s="1" t="s">
         <v>410</v>
       </c>
-      <c r="H85" s="16" t="s">
+      <c r="H85" s="1" t="s">
         <v>411</v>
       </c>
-      <c r="I85" s="15" t="s">
+      <c r="I85" s="12" t="s">
         <v>412</v>
       </c>
-      <c r="J85" s="16">
+      <c r="J85" s="1">
         <v>30</v>
       </c>
-      <c r="K85" t="str">
+      <c r="K85" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Dreamcast - Shenmue - Gold.jpg</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
-      <c r="A86" s="15" t="s">
+    <row r="86" s="1" customFormat="1" spans="1:11">
+      <c r="A86" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C86" s="7" t="s">
+      <c r="C86" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D86" s="7" t="s">
+      <c r="D86" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="E86" s="1" t="s">
         <v>415</v>
       </c>
-      <c r="F86" s="17">
+      <c r="F86" s="1">
         <v>150</v>
       </c>
-      <c r="G86" s="16" t="s">
+      <c r="G86" s="1" t="s">
         <v>416</v>
       </c>
-      <c r="H86" s="16" t="s">
+      <c r="H86" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I86" s="15" t="s">
+      <c r="I86" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="J86" s="16">
+      <c r="J86" s="1">
         <v>0</v>
       </c>
-      <c r="K86" t="str">
+      <c r="K86" s="1" t="str">
         <f t="shared" si="2"/>
         <v>_Gamecube - Console - Silver.jpg</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
-      <c r="A87" s="15" t="s">
+    <row r="87" s="1" customFormat="1" spans="1:11">
+      <c r="A87" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C87" s="7" t="s">
+      <c r="C87" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D87" s="7" t="s">
+      <c r="D87" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="E87" s="16" t="s">
+      <c r="E87" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="F87" s="17">
+      <c r="F87" s="1">
         <v>150</v>
       </c>
-      <c r="G87" s="16" t="s">
+      <c r="G87" s="1" t="s">
         <v>420</v>
       </c>
-      <c r="H87" s="16" t="s">
+      <c r="H87" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I87" s="15" t="s">
+      <c r="I87" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="J87" s="16">
+      <c r="J87" s="1">
         <v>-80</v>
       </c>
-      <c r="K87" t="str">
+      <c r="K87" s="1" t="str">
         <f t="shared" si="2"/>
         <v>_Gamecube - Console - Bronze.jpg</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
-      <c r="A88" s="15" t="s">
+    <row r="88" s="1" customFormat="1" spans="1:11">
+      <c r="A88" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C88" s="7" t="s">
+      <c r="C88" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D88" s="7" t="s">
+      <c r="D88" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E88" s="16" t="s">
+      <c r="E88" s="1" t="s">
         <v>421</v>
       </c>
-      <c r="F88" s="17">
+      <c r="F88" s="1">
         <v>150</v>
       </c>
-      <c r="G88" s="16" t="s">
+      <c r="G88" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="H88" s="16" t="s">
+      <c r="H88" s="1" t="s">
         <v>417</v>
       </c>
-      <c r="I88" s="15" t="s">
+      <c r="I88" s="12" t="s">
         <v>418</v>
       </c>
-      <c r="J88" s="16">
+      <c r="J88" s="1">
         <v>40</v>
       </c>
-      <c r="K88" t="str">
+      <c r="K88" s="1" t="str">
         <f t="shared" si="2"/>
         <v>_Gamecube - Console - Gold.jpg</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
-      <c r="A89" s="15" t="s">
+    <row r="89" s="1" customFormat="1" spans="1:11">
+      <c r="A89" s="12" t="s">
         <v>423</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C89" s="7" t="s">
+      <c r="C89" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D89" s="7" t="s">
+      <c r="D89" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E89" s="16" t="s">
+      <c r="E89" s="1" t="s">
         <v>424</v>
       </c>
-      <c r="F89" s="17">
+      <c r="F89" s="1">
         <v>45</v>
       </c>
-      <c r="G89" s="16" t="s">
+      <c r="G89" s="1" t="s">
         <v>425</v>
       </c>
-      <c r="H89" s="16" t="s">
+      <c r="H89" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="I89" s="15" t="s">
+      <c r="I89" s="12" t="s">
         <v>427</v>
       </c>
-      <c r="J89" s="16">
+      <c r="J89" s="1">
         <v>30</v>
       </c>
-      <c r="K89" t="str">
+      <c r="K89" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Gamecube - Super Smash Bros. Melee - Gold.jpg</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
-      <c r="A90" s="15" t="s">
+    <row r="90" s="1" customFormat="1" spans="1:11">
+      <c r="A90" s="12" t="s">
         <v>428</v>
       </c>
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="1" t="s">
         <v>414</v>
       </c>
-      <c r="C90" s="7" t="s">
+      <c r="C90" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D90" s="7" t="s">
+      <c r="D90" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E90" s="16" t="s">
+      <c r="E90" s="1" t="s">
         <v>429</v>
       </c>
-      <c r="F90" s="17">
+      <c r="F90" s="1">
         <v>35</v>
       </c>
-      <c r="G90" s="16" t="s">
+      <c r="G90" s="1" t="s">
         <v>430</v>
       </c>
-      <c r="H90" s="16" t="s">
+      <c r="H90" s="1" t="s">
         <v>431</v>
       </c>
-      <c r="I90" s="15" t="s">
+      <c r="I90" s="12" t="s">
         <v>432</v>
       </c>
-      <c r="J90" s="16">
+      <c r="J90" s="1">
         <v>25</v>
       </c>
-      <c r="K90" t="str">
+      <c r="K90" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Gamecube - Mario Party 4 - Gold.jpg</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
-      <c r="A91" s="15" t="s">
+    <row r="91" s="1" customFormat="1" spans="1:11">
+      <c r="A91" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C91" s="7" t="s">
+      <c r="C91" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="D91" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E91" s="16" t="s">
+      <c r="E91" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="F91" s="17">
+      <c r="F91" s="1">
         <v>120</v>
       </c>
-      <c r="G91" s="16" t="s">
+      <c r="G91" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="H91" s="16" t="s">
+      <c r="H91" s="1" t="s">
         <v>437</v>
       </c>
-      <c r="I91" s="15" t="s">
+      <c r="I91" s="12" t="s">
         <v>438</v>
       </c>
-      <c r="J91" s="16">
+      <c r="J91" s="1">
         <v>0</v>
       </c>
-      <c r="K91" t="str">
+      <c r="K91" s="1" t="str">
         <f t="shared" si="2"/>
         <v>_Playstation 2 - Console - Silver.jpg</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
-      <c r="A92" s="15" t="s">
+    <row r="92" s="1" customFormat="1" spans="1:11">
+      <c r="A92" s="12" t="s">
         <v>439</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="B92" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C92" s="7" t="s">
+      <c r="C92" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D92" s="7" t="s">
+      <c r="D92" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E92" s="16" t="s">
+      <c r="E92" s="1" t="s">
         <v>440</v>
       </c>
-      <c r="F92" s="17">
+      <c r="F92" s="1">
         <v>45</v>
       </c>
-      <c r="G92" s="16" t="s">
+      <c r="G92" s="1" t="s">
         <v>441</v>
       </c>
-      <c r="H92" s="16" t="s">
+      <c r="H92" s="1" t="s">
         <v>442</v>
       </c>
-      <c r="I92" s="15" t="s">
+      <c r="I92" s="12" t="s">
         <v>443</v>
       </c>
-      <c r="J92" s="16">
+      <c r="J92" s="1">
         <v>25</v>
       </c>
-      <c r="K92" t="str">
+      <c r="K92" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Playstation 2 - Boogie - Gold.jpg</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
-      <c r="A93" s="15" t="s">
+    <row r="93" s="1" customFormat="1" spans="1:11">
+      <c r="A93" s="12" t="s">
         <v>444</v>
       </c>
-      <c r="B93" s="16" t="s">
+      <c r="B93" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C93" s="7" t="s">
+      <c r="C93" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D93" s="7" t="s">
+      <c r="D93" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="E93" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="F93" s="17">
+      <c r="F93" s="1">
         <v>65</v>
       </c>
-      <c r="G93" s="16" t="s">
+      <c r="G93" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="H93" s="16" t="s">
+      <c r="H93" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="I93" s="15" t="s">
+      <c r="I93" s="12" t="s">
         <v>448</v>
       </c>
-      <c r="J93" s="16">
+      <c r="J93" s="1">
         <v>0</v>
       </c>
-      <c r="K93" t="str">
+      <c r="K93" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Playstation 2 - Dragon Quest L'Odyssée Du Roi Maudit - Silver.jpg</v>
       </c>
     </row>
-    <row r="94" spans="1:11">
-      <c r="A94" s="15" t="s">
+    <row r="94" s="1" customFormat="1" spans="1:11">
+      <c r="A94" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="B94" s="16" t="s">
+      <c r="B94" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C94" s="7" t="s">
+      <c r="C94" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D94" s="7" t="s">
+      <c r="D94" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="F94" s="17">
+      <c r="F94" s="1">
         <v>50</v>
       </c>
-      <c r="G94" s="16" t="s">
+      <c r="G94" s="1" t="s">
         <v>451</v>
       </c>
-      <c r="H94" s="16" t="s">
+      <c r="H94" s="1" t="s">
         <v>452</v>
       </c>
-      <c r="I94" s="15" t="s">
+      <c r="I94" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="J94" s="16">
+      <c r="J94" s="1">
         <v>100</v>
       </c>
-      <c r="K94" t="str">
+      <c r="K94" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Playstation 2 - Fifa 11 - Platinum.jpg</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
-      <c r="A95" s="15" t="s">
+    <row r="95" s="1" customFormat="1" spans="1:11">
+      <c r="A95" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="B95" s="16" t="s">
+      <c r="B95" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="C95" s="7" t="s">
+      <c r="C95" s="5" t="s">
         <v>376</v>
       </c>
-      <c r="D95" s="7" t="s">
+      <c r="D95" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E95" s="1" t="s">
         <v>455</v>
       </c>
-      <c r="F95" s="17">
+      <c r="F95" s="1">
         <v>60</v>
       </c>
-      <c r="G95" s="16" t="s">
+      <c r="G95" s="1" t="s">
         <v>456</v>
       </c>
-      <c r="H95" s="16" t="s">
+      <c r="H95" s="1" t="s">
         <v>457</v>
       </c>
-      <c r="I95" s="15" t="s">
+      <c r="I95" s="12" t="s">
         <v>458</v>
       </c>
-      <c r="J95" s="16">
+      <c r="J95" s="1">
         <v>0</v>
       </c>
-      <c r="K95" t="str">
+      <c r="K95" s="1" t="str">
         <f t="shared" si="2"/>
         <v>Playstation 2 - GTA Vice City - Silver.jpg</v>
       </c>

</xml_diff>